<commit_message>
test 1 plots changes
</commit_message>
<xml_diff>
--- a/challenge_response/variant-3/plots/test_1/alpha_large/conf_trust_0-2.xlsx
+++ b/challenge_response/variant-3/plots/test_1/alpha_large/conf_trust_0-2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H358"/>
+  <dimension ref="A1:H316"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,7 +503,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.008020334067243199</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -529,7 +529,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -555,7 +555,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
@@ -581,28 +581,28 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3</v>
+        <v>3.208010167033622</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -616,7 +616,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
@@ -633,10 +633,10 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>3.208010167033622</v>
+        <v>4</v>
       </c>
       <c r="B8" t="n">
-        <v>20</v>
+        <v>19.21603050110086</v>
       </c>
       <c r="C8" t="n">
         <v>1</v>
@@ -659,10 +659,10 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3.216030501100865</v>
+        <v>5</v>
       </c>
       <c r="B9" t="n">
-        <v>20</v>
+        <v>18.21603050110086</v>
       </c>
       <c r="C9" t="n">
         <v>1</v>
@@ -685,10 +685,10 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3.208010167033622</v>
+        <v>6</v>
       </c>
       <c r="B10" t="n">
-        <v>20</v>
+        <v>17.21603050110086</v>
       </c>
       <c r="C10" t="n">
         <v>1</v>
@@ -711,10 +711,10 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B11" t="n">
-        <v>19.21603050110086</v>
+        <v>16.21603050110086</v>
       </c>
       <c r="C11" t="n">
         <v>1</v>
@@ -737,10 +737,10 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B12" t="n">
-        <v>18.21603050110086</v>
+        <v>15.21603050110086</v>
       </c>
       <c r="C12" t="n">
         <v>1</v>
@@ -763,10 +763,10 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B13" t="n">
-        <v>17.21603050110086</v>
+        <v>14.21603050110086</v>
       </c>
       <c r="C13" t="n">
         <v>1</v>
@@ -789,10 +789,10 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B14" t="n">
-        <v>16.21603050110086</v>
+        <v>13.21603050110086</v>
       </c>
       <c r="C14" t="n">
         <v>1</v>
@@ -815,10 +815,10 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B15" t="n">
-        <v>15.21603050110086</v>
+        <v>12.21603050110086</v>
       </c>
       <c r="C15" t="n">
         <v>1</v>
@@ -841,10 +841,10 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B16" t="n">
-        <v>14.21603050110086</v>
+        <v>11.21603050110086</v>
       </c>
       <c r="C16" t="n">
         <v>1</v>
@@ -867,10 +867,10 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B17" t="n">
-        <v>13.21603050110086</v>
+        <v>10.21603050110086</v>
       </c>
       <c r="C17" t="n">
         <v>1</v>
@@ -893,10 +893,10 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B18" t="n">
-        <v>12.21603050110086</v>
+        <v>9.216030501100864</v>
       </c>
       <c r="C18" t="n">
         <v>1</v>
@@ -919,10 +919,10 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B19" t="n">
-        <v>11.21603050110086</v>
+        <v>20</v>
       </c>
       <c r="C19" t="n">
         <v>1</v>
@@ -945,10 +945,10 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>13</v>
+        <v>15.00802033406724</v>
       </c>
       <c r="B20" t="n">
-        <v>10.21603050110086</v>
+        <v>20</v>
       </c>
       <c r="C20" t="n">
         <v>1</v>
@@ -971,10 +971,10 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B21" t="n">
-        <v>9.216030501100864</v>
+        <v>19</v>
       </c>
       <c r="C21" t="n">
         <v>1</v>
@@ -997,10 +997,10 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>15.00802033406724</v>
+        <v>17</v>
       </c>
       <c r="B22" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C22" t="n">
         <v>1</v>
@@ -1023,10 +1023,10 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B23" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C23" t="n">
         <v>1</v>
@@ -1049,10 +1049,10 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>15.00802033406724</v>
+        <v>19</v>
       </c>
       <c r="B24" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C24" t="n">
         <v>1</v>
@@ -1075,10 +1075,10 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
+        <v>20</v>
+      </c>
+      <c r="B25" t="n">
         <v>15</v>
-      </c>
-      <c r="B25" t="n">
-        <v>20</v>
       </c>
       <c r="C25" t="n">
         <v>1</v>
@@ -1101,10 +1101,10 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B26" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C26" t="n">
         <v>1</v>
@@ -1127,10 +1127,10 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B27" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C27" t="n">
         <v>1</v>
@@ -1153,10 +1153,10 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B28" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C28" t="n">
         <v>1</v>
@@ -1179,10 +1179,10 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B29" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C29" t="n">
         <v>1</v>
@@ -1205,10 +1205,10 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B30" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C30" t="n">
         <v>1</v>
@@ -1231,10 +1231,10 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B31" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C31" t="n">
         <v>1</v>
@@ -1257,10 +1257,10 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B32" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C32" t="n">
         <v>1</v>
@@ -1283,10 +1283,10 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B33" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C33" t="n">
         <v>1</v>
@@ -1309,10 +1309,10 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B34" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C34" t="n">
         <v>1</v>
@@ -1335,10 +1335,10 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B35" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C35" t="n">
         <v>1</v>
@@ -1361,10 +1361,10 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>25</v>
+        <v>30.00802033406724</v>
       </c>
       <c r="B36" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C36" t="n">
         <v>1</v>
@@ -1387,10 +1387,10 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B37" t="n">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C37" t="n">
         <v>1</v>
@@ -1413,10 +1413,10 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B38" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C38" t="n">
         <v>1</v>
@@ -1439,10 +1439,10 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B39" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C39" t="n">
         <v>1</v>
@@ -1465,10 +1465,10 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>29</v>
+        <v>33.20801016703362</v>
       </c>
       <c r="B40" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C40" t="n">
         <v>1</v>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>30.00802033406724</v>
+        <v>33.21603050110087</v>
       </c>
       <c r="B41" t="n">
         <v>20</v>
@@ -1517,7 +1517,7 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>30</v>
+        <v>33.22405083516811</v>
       </c>
       <c r="B42" t="n">
         <v>20</v>
@@ -1543,10 +1543,10 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>30.00802033406724</v>
+        <v>34</v>
       </c>
       <c r="B43" t="n">
-        <v>20</v>
+        <v>19.22405083516811</v>
       </c>
       <c r="C43" t="n">
         <v>1</v>
@@ -1569,10 +1569,10 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B44" t="n">
-        <v>20</v>
+        <v>18.22405083516811</v>
       </c>
       <c r="C44" t="n">
         <v>1</v>
@@ -1595,10 +1595,10 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B45" t="n">
-        <v>20</v>
+        <v>17.22405083516811</v>
       </c>
       <c r="C45" t="n">
         <v>1</v>
@@ -1621,10 +1621,10 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B46" t="n">
-        <v>19</v>
+        <v>16.22405083516811</v>
       </c>
       <c r="C46" t="n">
         <v>1</v>
@@ -1647,10 +1647,10 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B47" t="n">
-        <v>18</v>
+        <v>15.22405083516811</v>
       </c>
       <c r="C47" t="n">
         <v>1</v>
@@ -1673,10 +1673,10 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B48" t="n">
-        <v>17</v>
+        <v>14.22405083516811</v>
       </c>
       <c r="C48" t="n">
         <v>1</v>
@@ -1699,10 +1699,10 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>33.21603050110087</v>
+        <v>40</v>
       </c>
       <c r="B49" t="n">
-        <v>20</v>
+        <v>13.22405083516811</v>
       </c>
       <c r="C49" t="n">
         <v>1</v>
@@ -1725,10 +1725,10 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>33.20801016703362</v>
+        <v>41</v>
       </c>
       <c r="B50" t="n">
-        <v>20</v>
+        <v>12.22405083516811</v>
       </c>
       <c r="C50" t="n">
         <v>1</v>
@@ -1751,10 +1751,10 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>33.21603050110087</v>
+        <v>42</v>
       </c>
       <c r="B51" t="n">
-        <v>20</v>
+        <v>11.22405083516811</v>
       </c>
       <c r="C51" t="n">
         <v>1</v>
@@ -1777,10 +1777,10 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>33.20801016703362</v>
+        <v>43</v>
       </c>
       <c r="B52" t="n">
-        <v>20</v>
+        <v>10.22405083516811</v>
       </c>
       <c r="C52" t="n">
         <v>1</v>
@@ -1803,10 +1803,10 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>33.22405083516811</v>
+        <v>44</v>
       </c>
       <c r="B53" t="n">
-        <v>20</v>
+        <v>9.224050835168114</v>
       </c>
       <c r="C53" t="n">
         <v>1</v>
@@ -1829,7 +1829,7 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>33.21603050110087</v>
+        <v>45</v>
       </c>
       <c r="B54" t="n">
         <v>20</v>
@@ -1855,10 +1855,10 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>34</v>
+        <v>45.00802033406725</v>
       </c>
       <c r="B55" t="n">
-        <v>19.22405083516811</v>
+        <v>20</v>
       </c>
       <c r="C55" t="n">
         <v>1</v>
@@ -1881,10 +1881,10 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B56" t="n">
-        <v>18.22405083516811</v>
+        <v>19</v>
       </c>
       <c r="C56" t="n">
         <v>1</v>
@@ -1907,10 +1907,10 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B57" t="n">
-        <v>17.22405083516811</v>
+        <v>18</v>
       </c>
       <c r="C57" t="n">
         <v>1</v>
@@ -1933,10 +1933,10 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B58" t="n">
-        <v>16.22405083516811</v>
+        <v>17</v>
       </c>
       <c r="C58" t="n">
         <v>1</v>
@@ -1959,10 +1959,10 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B59" t="n">
-        <v>15.22405083516811</v>
+        <v>16</v>
       </c>
       <c r="C59" t="n">
         <v>1</v>
@@ -1985,10 +1985,10 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B60" t="n">
-        <v>14.22405083516811</v>
+        <v>15</v>
       </c>
       <c r="C60" t="n">
         <v>1</v>
@@ -2011,10 +2011,10 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B61" t="n">
-        <v>13.22405083516811</v>
+        <v>14</v>
       </c>
       <c r="C61" t="n">
         <v>1</v>
@@ -2037,10 +2037,10 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B62" t="n">
-        <v>12.22405083516811</v>
+        <v>13</v>
       </c>
       <c r="C62" t="n">
         <v>1</v>
@@ -2063,10 +2063,10 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B63" t="n">
-        <v>11.22405083516811</v>
+        <v>12</v>
       </c>
       <c r="C63" t="n">
         <v>1</v>
@@ -2089,10 +2089,10 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B64" t="n">
-        <v>10.22405083516811</v>
+        <v>11</v>
       </c>
       <c r="C64" t="n">
         <v>1</v>
@@ -2115,10 +2115,10 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B65" t="n">
-        <v>9.224050835168114</v>
+        <v>10</v>
       </c>
       <c r="C65" t="n">
         <v>1</v>
@@ -2141,10 +2141,10 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>45.00802033406725</v>
+        <v>56</v>
       </c>
       <c r="B66" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C66" t="n">
         <v>1</v>
@@ -2167,10 +2167,10 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B67" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C67" t="n">
         <v>1</v>
@@ -2193,10 +2193,10 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>45.00802033406725</v>
+        <v>58</v>
       </c>
       <c r="B68" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C68" t="n">
         <v>1</v>
@@ -2219,10 +2219,10 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B69" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C69" t="n">
         <v>1</v>
@@ -2245,7 +2245,7 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="B70" t="n">
         <v>20</v>
@@ -2271,10 +2271,10 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>46</v>
+        <v>60.00802033406725</v>
       </c>
       <c r="B71" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C71" t="n">
         <v>1</v>
@@ -2297,10 +2297,10 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="B72" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C72" t="n">
         <v>1</v>
@@ -2323,10 +2323,10 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B73" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C73" t="n">
         <v>1</v>
@@ -2349,10 +2349,10 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B74" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C74" t="n">
         <v>1</v>
@@ -2375,10 +2375,10 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>50</v>
+        <v>63.20801016703363</v>
       </c>
       <c r="B75" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C75" t="n">
         <v>1</v>
@@ -2401,10 +2401,10 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>51</v>
+        <v>63.21603050110088</v>
       </c>
       <c r="B76" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C76" t="n">
         <v>1</v>
@@ -2427,10 +2427,10 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>52</v>
+        <v>63.22405083516812</v>
       </c>
       <c r="B77" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C77" t="n">
         <v>1</v>
@@ -2453,10 +2453,10 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B78" t="n">
-        <v>12</v>
+        <v>19.22405083516812</v>
       </c>
       <c r="C78" t="n">
         <v>1</v>
@@ -2479,10 +2479,10 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B79" t="n">
-        <v>11</v>
+        <v>18.22405083516812</v>
       </c>
       <c r="C79" t="n">
         <v>1</v>
@@ -2505,10 +2505,10 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B80" t="n">
-        <v>10</v>
+        <v>17.22405083516812</v>
       </c>
       <c r="C80" t="n">
         <v>1</v>
@@ -2531,10 +2531,10 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B81" t="n">
-        <v>9</v>
+        <v>16.22405083516812</v>
       </c>
       <c r="C81" t="n">
         <v>1</v>
@@ -2557,10 +2557,10 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B82" t="n">
-        <v>8</v>
+        <v>15.22405083516812</v>
       </c>
       <c r="C82" t="n">
         <v>1</v>
@@ -2583,10 +2583,10 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B83" t="n">
-        <v>7</v>
+        <v>14.22405083516812</v>
       </c>
       <c r="C83" t="n">
         <v>1</v>
@@ -2609,10 +2609,10 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B84" t="n">
-        <v>6</v>
+        <v>13.22405083516812</v>
       </c>
       <c r="C84" t="n">
         <v>1</v>
@@ -2635,10 +2635,10 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>60.00802033406725</v>
+        <v>71</v>
       </c>
       <c r="B85" t="n">
-        <v>20</v>
+        <v>12.22405083516812</v>
       </c>
       <c r="C85" t="n">
         <v>1</v>
@@ -2661,10 +2661,10 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B86" t="n">
-        <v>20</v>
+        <v>11.22405083516812</v>
       </c>
       <c r="C86" t="n">
         <v>1</v>
@@ -2687,10 +2687,10 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>60.00802033406725</v>
+        <v>73</v>
       </c>
       <c r="B87" t="n">
-        <v>20</v>
+        <v>10.22405083516812</v>
       </c>
       <c r="C87" t="n">
         <v>1</v>
@@ -2713,10 +2713,10 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B88" t="n">
-        <v>20</v>
+        <v>9.22405083516812</v>
       </c>
       <c r="C88" t="n">
         <v>1</v>
@@ -2739,7 +2739,7 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B89" t="n">
         <v>20</v>
@@ -2765,10 +2765,10 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>61</v>
+        <v>75.00802033406724</v>
       </c>
       <c r="B90" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C90" t="n">
         <v>1</v>
@@ -2791,10 +2791,10 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="B91" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C91" t="n">
         <v>1</v>
@@ -2817,10 +2817,10 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="B92" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C92" t="n">
         <v>1</v>
@@ -2843,10 +2843,10 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>63.21603050110088</v>
+        <v>78</v>
       </c>
       <c r="B93" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C93" t="n">
         <v>1</v>
@@ -2869,10 +2869,10 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>63.20801016703363</v>
+        <v>79</v>
       </c>
       <c r="B94" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C94" t="n">
         <v>1</v>
@@ -2895,10 +2895,10 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>63.21603050110088</v>
+        <v>80</v>
       </c>
       <c r="B95" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C95" t="n">
         <v>1</v>
@@ -2921,10 +2921,10 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>63.20801016703363</v>
+        <v>81</v>
       </c>
       <c r="B96" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C96" t="n">
         <v>1</v>
@@ -2947,10 +2947,10 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>63.22405083516812</v>
+        <v>82</v>
       </c>
       <c r="B97" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C97" t="n">
         <v>1</v>
@@ -2973,10 +2973,10 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>63.21603050110088</v>
+        <v>83</v>
       </c>
       <c r="B98" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C98" t="n">
         <v>1</v>
@@ -2999,10 +2999,10 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="B99" t="n">
-        <v>19.22405083516812</v>
+        <v>11</v>
       </c>
       <c r="C99" t="n">
         <v>1</v>
@@ -3025,10 +3025,10 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="B100" t="n">
-        <v>18.22405083516812</v>
+        <v>10</v>
       </c>
       <c r="C100" t="n">
         <v>1</v>
@@ -3051,10 +3051,10 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="B101" t="n">
-        <v>17.22405083516812</v>
+        <v>9</v>
       </c>
       <c r="C101" t="n">
         <v>1</v>
@@ -3077,10 +3077,10 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="B102" t="n">
-        <v>16.22405083516812</v>
+        <v>8</v>
       </c>
       <c r="C102" t="n">
         <v>1</v>
@@ -3103,10 +3103,10 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="B103" t="n">
-        <v>15.22405083516812</v>
+        <v>7</v>
       </c>
       <c r="C103" t="n">
         <v>1</v>
@@ -3129,10 +3129,10 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="B104" t="n">
-        <v>14.22405083516812</v>
+        <v>6</v>
       </c>
       <c r="C104" t="n">
         <v>1</v>
@@ -3155,10 +3155,10 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="B105" t="n">
-        <v>13.22405083516812</v>
+        <v>20</v>
       </c>
       <c r="C105" t="n">
         <v>1</v>
@@ -3181,10 +3181,10 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>71</v>
+        <v>90.00802033406724</v>
       </c>
       <c r="B106" t="n">
-        <v>12.22405083516812</v>
+        <v>20</v>
       </c>
       <c r="C106" t="n">
         <v>1</v>
@@ -3207,10 +3207,10 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="B107" t="n">
-        <v>11.22405083516812</v>
+        <v>19</v>
       </c>
       <c r="C107" t="n">
         <v>1</v>
@@ -3233,10 +3233,10 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="B108" t="n">
-        <v>10.22405083516812</v>
+        <v>18</v>
       </c>
       <c r="C108" t="n">
         <v>1</v>
@@ -3259,10 +3259,10 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="B109" t="n">
-        <v>9.22405083516812</v>
+        <v>17</v>
       </c>
       <c r="C109" t="n">
         <v>1</v>
@@ -3285,7 +3285,7 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>75.00802033406724</v>
+        <v>93.20801016703362</v>
       </c>
       <c r="B110" t="n">
         <v>20</v>
@@ -3311,7 +3311,7 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>75</v>
+        <v>93.21603050110086</v>
       </c>
       <c r="B111" t="n">
         <v>20</v>
@@ -3337,7 +3337,7 @@
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>75.00802033406724</v>
+        <v>93.2240508351681</v>
       </c>
       <c r="B112" t="n">
         <v>20</v>
@@ -3363,10 +3363,10 @@
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="B113" t="n">
-        <v>20</v>
+        <v>19.2240508351681</v>
       </c>
       <c r="C113" t="n">
         <v>1</v>
@@ -3389,10 +3389,10 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="B114" t="n">
-        <v>20</v>
+        <v>18.2240508351681</v>
       </c>
       <c r="C114" t="n">
         <v>1</v>
@@ -3415,10 +3415,10 @@
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="B115" t="n">
-        <v>19</v>
+        <v>17.2240508351681</v>
       </c>
       <c r="C115" t="n">
         <v>1</v>
@@ -3441,10 +3441,10 @@
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="B116" t="n">
-        <v>18</v>
+        <v>16.2240508351681</v>
       </c>
       <c r="C116" t="n">
         <v>1</v>
@@ -3467,10 +3467,10 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="B117" t="n">
-        <v>17</v>
+        <v>15.2240508351681</v>
       </c>
       <c r="C117" t="n">
         <v>1</v>
@@ -3493,10 +3493,10 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="B118" t="n">
-        <v>16</v>
+        <v>14.2240508351681</v>
       </c>
       <c r="C118" t="n">
         <v>1</v>
@@ -3519,10 +3519,10 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="B119" t="n">
-        <v>15</v>
+        <v>13.2240508351681</v>
       </c>
       <c r="C119" t="n">
         <v>1</v>
@@ -3545,10 +3545,10 @@
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="B120" t="n">
-        <v>14</v>
+        <v>12.2240508351681</v>
       </c>
       <c r="C120" t="n">
         <v>1</v>
@@ -3571,10 +3571,10 @@
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="B121" t="n">
-        <v>13</v>
+        <v>11.2240508351681</v>
       </c>
       <c r="C121" t="n">
         <v>1</v>
@@ -3597,10 +3597,10 @@
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="B122" t="n">
-        <v>12</v>
+        <v>10.2240508351681</v>
       </c>
       <c r="C122" t="n">
         <v>1</v>
@@ -3623,10 +3623,10 @@
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="B123" t="n">
-        <v>11</v>
+        <v>9.2240508351681</v>
       </c>
       <c r="C123" t="n">
         <v>1</v>
@@ -3649,10 +3649,10 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="B124" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C124" t="n">
         <v>1</v>
@@ -3675,10 +3675,10 @@
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>86</v>
+        <v>105.0080203340672</v>
       </c>
       <c r="B125" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C125" t="n">
         <v>1</v>
@@ -3701,10 +3701,10 @@
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="B126" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C126" t="n">
         <v>1</v>
@@ -3727,10 +3727,10 @@
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="B127" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C127" t="n">
         <v>1</v>
@@ -3753,10 +3753,10 @@
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="B128" t="n">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C128" t="n">
         <v>1</v>
@@ -3779,10 +3779,10 @@
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>90.00802033406724</v>
+        <v>109</v>
       </c>
       <c r="B129" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C129" t="n">
         <v>1</v>
@@ -3805,10 +3805,10 @@
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="B130" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C130" t="n">
         <v>1</v>
@@ -3831,10 +3831,10 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>90.00802033406724</v>
+        <v>111</v>
       </c>
       <c r="B131" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C131" t="n">
         <v>1</v>
@@ -3857,10 +3857,10 @@
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="B132" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C132" t="n">
         <v>1</v>
@@ -3883,10 +3883,10 @@
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="B133" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C133" t="n">
         <v>1</v>
@@ -3909,10 +3909,10 @@
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="B134" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C134" t="n">
         <v>1</v>
@@ -3935,10 +3935,10 @@
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="B135" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C135" t="n">
         <v>1</v>
@@ -3961,10 +3961,10 @@
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="B136" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C136" t="n">
         <v>1</v>
@@ -3987,10 +3987,10 @@
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>93.21603050110086</v>
+        <v>117</v>
       </c>
       <c r="B137" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C137" t="n">
         <v>1</v>
@@ -4013,10 +4013,10 @@
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>93.20801016703362</v>
+        <v>118</v>
       </c>
       <c r="B138" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C138" t="n">
         <v>1</v>
@@ -4039,10 +4039,10 @@
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>93.21603050110086</v>
+        <v>119</v>
       </c>
       <c r="B139" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C139" t="n">
         <v>1</v>
@@ -4065,7 +4065,7 @@
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>93.20801016703362</v>
+        <v>120</v>
       </c>
       <c r="B140" t="n">
         <v>20</v>
@@ -4091,7 +4091,7 @@
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>93.2240508351681</v>
+        <v>120.0080203340672</v>
       </c>
       <c r="B141" t="n">
         <v>20</v>
@@ -4117,10 +4117,10 @@
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>93.21603050110086</v>
+        <v>121</v>
       </c>
       <c r="B142" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C142" t="n">
         <v>1</v>
@@ -4143,10 +4143,10 @@
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="B143" t="n">
-        <v>19.2240508351681</v>
+        <v>18</v>
       </c>
       <c r="C143" t="n">
         <v>1</v>
@@ -4169,10 +4169,10 @@
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="B144" t="n">
-        <v>18.2240508351681</v>
+        <v>17</v>
       </c>
       <c r="C144" t="n">
         <v>1</v>
@@ -4195,10 +4195,10 @@
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>96</v>
+        <v>123.2080101670336</v>
       </c>
       <c r="B145" t="n">
-        <v>17.2240508351681</v>
+        <v>20</v>
       </c>
       <c r="C145" t="n">
         <v>1</v>
@@ -4221,10 +4221,10 @@
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>97</v>
+        <v>123.2160305011009</v>
       </c>
       <c r="B146" t="n">
-        <v>16.2240508351681</v>
+        <v>20</v>
       </c>
       <c r="C146" t="n">
         <v>1</v>
@@ -4247,10 +4247,10 @@
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>98</v>
+        <v>123.2240508351681</v>
       </c>
       <c r="B147" t="n">
-        <v>15.2240508351681</v>
+        <v>20</v>
       </c>
       <c r="C147" t="n">
         <v>1</v>
@@ -4273,10 +4273,10 @@
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="B148" t="n">
-        <v>14.2240508351681</v>
+        <v>19.2240508351681</v>
       </c>
       <c r="C148" t="n">
         <v>1</v>
@@ -4299,10 +4299,10 @@
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="B149" t="n">
-        <v>13.2240508351681</v>
+        <v>18.2240508351681</v>
       </c>
       <c r="C149" t="n">
         <v>1</v>
@@ -4325,10 +4325,10 @@
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="B150" t="n">
-        <v>12.2240508351681</v>
+        <v>17.2240508351681</v>
       </c>
       <c r="C150" t="n">
         <v>1</v>
@@ -4351,10 +4351,10 @@
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="B151" t="n">
-        <v>11.2240508351681</v>
+        <v>16.2240508351681</v>
       </c>
       <c r="C151" t="n">
         <v>1</v>
@@ -4377,10 +4377,10 @@
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="B152" t="n">
-        <v>10.2240508351681</v>
+        <v>15.2240508351681</v>
       </c>
       <c r="C152" t="n">
         <v>1</v>
@@ -4403,10 +4403,10 @@
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="B153" t="n">
-        <v>9.2240508351681</v>
+        <v>14.2240508351681</v>
       </c>
       <c r="C153" t="n">
         <v>1</v>
@@ -4429,10 +4429,10 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>105.0080203340672</v>
+        <v>130</v>
       </c>
       <c r="B154" t="n">
-        <v>20</v>
+        <v>13.2240508351681</v>
       </c>
       <c r="C154" t="n">
         <v>1</v>
@@ -4455,10 +4455,10 @@
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B155" t="n">
-        <v>20</v>
+        <v>12.2240508351681</v>
       </c>
       <c r="C155" t="n">
         <v>1</v>
@@ -4481,10 +4481,10 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>105.0080203340672</v>
+        <v>132</v>
       </c>
       <c r="B156" t="n">
-        <v>20</v>
+        <v>11.2240508351681</v>
       </c>
       <c r="C156" t="n">
         <v>1</v>
@@ -4507,10 +4507,10 @@
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="B157" t="n">
-        <v>20</v>
+        <v>10.2240508351681</v>
       </c>
       <c r="C157" t="n">
         <v>1</v>
@@ -4533,10 +4533,10 @@
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="B158" t="n">
-        <v>20</v>
+        <v>9.2240508351681</v>
       </c>
       <c r="C158" t="n">
         <v>1</v>
@@ -4559,10 +4559,10 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="B159" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C159" t="n">
         <v>1</v>
@@ -4585,10 +4585,10 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>107</v>
+        <v>135.0080203340673</v>
       </c>
       <c r="B160" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C160" t="n">
         <v>1</v>
@@ -4611,10 +4611,10 @@
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>108</v>
+        <v>136</v>
       </c>
       <c r="B161" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C161" t="n">
         <v>1</v>
@@ -4637,10 +4637,10 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>109</v>
+        <v>137</v>
       </c>
       <c r="B162" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C162" t="n">
         <v>1</v>
@@ -4663,10 +4663,10 @@
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="B163" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C163" t="n">
         <v>1</v>
@@ -4689,10 +4689,10 @@
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="B164" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C164" t="n">
         <v>1</v>
@@ -4715,10 +4715,10 @@
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="B165" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C165" t="n">
         <v>1</v>
@@ -4741,10 +4741,10 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>113</v>
+        <v>141</v>
       </c>
       <c r="B166" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C166" t="n">
         <v>1</v>
@@ -4767,10 +4767,10 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>114</v>
+        <v>142</v>
       </c>
       <c r="B167" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C167" t="n">
         <v>1</v>
@@ -4793,10 +4793,10 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="B168" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C168" t="n">
         <v>1</v>
@@ -4819,10 +4819,10 @@
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="B169" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C169" t="n">
         <v>1</v>
@@ -4845,10 +4845,10 @@
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="B170" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C170" t="n">
         <v>1</v>
@@ -4871,10 +4871,10 @@
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="B171" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C171" t="n">
         <v>1</v>
@@ -4897,10 +4897,10 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>119</v>
+        <v>147</v>
       </c>
       <c r="B172" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C172" t="n">
         <v>1</v>
@@ -4923,10 +4923,10 @@
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>120.0080203340672</v>
+        <v>148</v>
       </c>
       <c r="B173" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C173" t="n">
         <v>1</v>
@@ -4949,10 +4949,10 @@
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>120</v>
+        <v>149</v>
       </c>
       <c r="B174" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C174" t="n">
         <v>1</v>
@@ -4975,10 +4975,10 @@
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>120.0080203340672</v>
+        <v>150</v>
       </c>
       <c r="B175" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C175" t="n">
         <v>1</v>
@@ -5001,10 +5001,10 @@
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>120</v>
+        <v>151</v>
       </c>
       <c r="B176" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C176" t="n">
         <v>1</v>
@@ -5027,10 +5027,10 @@
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="B177" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C177" t="n">
         <v>1</v>
@@ -5053,10 +5053,10 @@
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="B178" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C178" t="n">
         <v>1</v>
@@ -5079,10 +5079,10 @@
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="B179" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C179" t="n">
         <v>1</v>
@@ -5105,10 +5105,10 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="B180" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C180" t="n">
         <v>1</v>
@@ -5131,10 +5131,10 @@
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>123.2160305011009</v>
+        <v>156</v>
       </c>
       <c r="B181" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C181" t="n">
         <v>1</v>
@@ -5157,10 +5157,10 @@
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>123.2080101670336</v>
+        <v>157</v>
       </c>
       <c r="B182" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C182" t="n">
         <v>1</v>
@@ -5183,10 +5183,10 @@
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>123.2160305011009</v>
+        <v>158</v>
       </c>
       <c r="B183" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C183" t="n">
         <v>1</v>
@@ -5209,10 +5209,10 @@
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>123.2080101670336</v>
+        <v>159</v>
       </c>
       <c r="B184" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C184" t="n">
         <v>1</v>
@@ -5235,10 +5235,10 @@
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>123.2240508351681</v>
+        <v>160</v>
       </c>
       <c r="B185" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C185" t="n">
         <v>1</v>
@@ -5261,10 +5261,10 @@
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>123.2160305011009</v>
+        <v>161</v>
       </c>
       <c r="B186" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C186" t="n">
         <v>1</v>
@@ -5287,10 +5287,10 @@
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>124</v>
+        <v>162</v>
       </c>
       <c r="B187" t="n">
-        <v>19.2240508351681</v>
+        <v>0</v>
       </c>
       <c r="C187" t="n">
         <v>1</v>
@@ -5313,10 +5313,10 @@
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>125</v>
+        <v>163</v>
       </c>
       <c r="B188" t="n">
-        <v>18.2240508351681</v>
+        <v>0</v>
       </c>
       <c r="C188" t="n">
         <v>1</v>
@@ -5339,10 +5339,10 @@
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>126</v>
+        <v>164</v>
       </c>
       <c r="B189" t="n">
-        <v>17.2240508351681</v>
+        <v>0</v>
       </c>
       <c r="C189" t="n">
         <v>1</v>
@@ -5365,10 +5365,10 @@
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="B190" t="n">
-        <v>16.2240508351681</v>
+        <v>0</v>
       </c>
       <c r="C190" t="n">
         <v>1</v>
@@ -5391,10 +5391,10 @@
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="B191" t="n">
-        <v>15.2240508351681</v>
+        <v>0</v>
       </c>
       <c r="C191" t="n">
         <v>1</v>
@@ -5417,10 +5417,10 @@
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="B192" t="n">
-        <v>14.2240508351681</v>
+        <v>0</v>
       </c>
       <c r="C192" t="n">
         <v>1</v>
@@ -5443,10 +5443,10 @@
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>130</v>
+        <v>168</v>
       </c>
       <c r="B193" t="n">
-        <v>13.2240508351681</v>
+        <v>0</v>
       </c>
       <c r="C193" t="n">
         <v>1</v>
@@ -5469,10 +5469,10 @@
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>131</v>
+        <v>169</v>
       </c>
       <c r="B194" t="n">
-        <v>12.2240508351681</v>
+        <v>0</v>
       </c>
       <c r="C194" t="n">
         <v>1</v>
@@ -5495,10 +5495,10 @@
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>132</v>
+        <v>170</v>
       </c>
       <c r="B195" t="n">
-        <v>11.2240508351681</v>
+        <v>0</v>
       </c>
       <c r="C195" t="n">
         <v>1</v>
@@ -5521,10 +5521,10 @@
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>133</v>
+        <v>171</v>
       </c>
       <c r="B196" t="n">
-        <v>10.2240508351681</v>
+        <v>0</v>
       </c>
       <c r="C196" t="n">
         <v>1</v>
@@ -5547,10 +5547,10 @@
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>134</v>
+        <v>172</v>
       </c>
       <c r="B197" t="n">
-        <v>9.2240508351681</v>
+        <v>0</v>
       </c>
       <c r="C197" t="n">
         <v>1</v>
@@ -5573,10 +5573,10 @@
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>135.0080203340673</v>
+        <v>173</v>
       </c>
       <c r="B198" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C198" t="n">
         <v>1</v>
@@ -5599,10 +5599,10 @@
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>135</v>
+        <v>174</v>
       </c>
       <c r="B199" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C199" t="n">
         <v>1</v>
@@ -5625,10 +5625,10 @@
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>135.0080203340673</v>
+        <v>175</v>
       </c>
       <c r="B200" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C200" t="n">
         <v>1</v>
@@ -5651,10 +5651,10 @@
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>135</v>
+        <v>176</v>
       </c>
       <c r="B201" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C201" t="n">
         <v>1</v>
@@ -5677,10 +5677,10 @@
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>135</v>
+        <v>177</v>
       </c>
       <c r="B202" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C202" t="n">
         <v>1</v>
@@ -5703,10 +5703,10 @@
     </row>
     <row r="203">
       <c r="A203" t="n">
-        <v>136</v>
+        <v>178</v>
       </c>
       <c r="B203" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C203" t="n">
         <v>1</v>
@@ -5729,10 +5729,10 @@
     </row>
     <row r="204">
       <c r="A204" t="n">
-        <v>137</v>
+        <v>179</v>
       </c>
       <c r="B204" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C204" t="n">
         <v>1</v>
@@ -5755,10 +5755,10 @@
     </row>
     <row r="205">
       <c r="A205" t="n">
-        <v>138</v>
+        <v>180</v>
       </c>
       <c r="B205" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C205" t="n">
         <v>1</v>
@@ -5781,10 +5781,10 @@
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>139</v>
+        <v>181</v>
       </c>
       <c r="B206" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C206" t="n">
         <v>1</v>
@@ -5807,10 +5807,10 @@
     </row>
     <row r="207">
       <c r="A207" t="n">
-        <v>140</v>
+        <v>182</v>
       </c>
       <c r="B207" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C207" t="n">
         <v>1</v>
@@ -5833,10 +5833,10 @@
     </row>
     <row r="208">
       <c r="A208" t="n">
-        <v>141</v>
+        <v>183</v>
       </c>
       <c r="B208" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C208" t="n">
         <v>1</v>
@@ -5859,10 +5859,10 @@
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>142</v>
+        <v>184</v>
       </c>
       <c r="B209" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C209" t="n">
         <v>1</v>
@@ -5885,10 +5885,10 @@
     </row>
     <row r="210">
       <c r="A210" t="n">
-        <v>143</v>
+        <v>185</v>
       </c>
       <c r="B210" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C210" t="n">
         <v>1</v>
@@ -5911,10 +5911,10 @@
     </row>
     <row r="211">
       <c r="A211" t="n">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="B211" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C211" t="n">
         <v>1</v>
@@ -5937,10 +5937,10 @@
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>145</v>
+        <v>187</v>
       </c>
       <c r="B212" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C212" t="n">
         <v>1</v>
@@ -5963,10 +5963,10 @@
     </row>
     <row r="213">
       <c r="A213" t="n">
-        <v>146</v>
+        <v>188</v>
       </c>
       <c r="B213" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C213" t="n">
         <v>1</v>
@@ -5989,10 +5989,10 @@
     </row>
     <row r="214">
       <c r="A214" t="n">
-        <v>147</v>
+        <v>189</v>
       </c>
       <c r="B214" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C214" t="n">
         <v>1</v>
@@ -6015,10 +6015,10 @@
     </row>
     <row r="215">
       <c r="A215" t="n">
-        <v>148</v>
+        <v>190</v>
       </c>
       <c r="B215" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C215" t="n">
         <v>1</v>
@@ -6041,10 +6041,10 @@
     </row>
     <row r="216">
       <c r="A216" t="n">
-        <v>149</v>
+        <v>191</v>
       </c>
       <c r="B216" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C216" t="n">
         <v>1</v>
@@ -6067,10 +6067,10 @@
     </row>
     <row r="217">
       <c r="A217" t="n">
-        <v>150</v>
+        <v>192</v>
       </c>
       <c r="B217" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C217" t="n">
         <v>1</v>
@@ -6093,10 +6093,10 @@
     </row>
     <row r="218">
       <c r="A218" t="n">
-        <v>151</v>
+        <v>193</v>
       </c>
       <c r="B218" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C218" t="n">
         <v>1</v>
@@ -6119,10 +6119,10 @@
     </row>
     <row r="219">
       <c r="A219" t="n">
-        <v>152</v>
+        <v>194</v>
       </c>
       <c r="B219" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C219" t="n">
         <v>1</v>
@@ -6145,10 +6145,10 @@
     </row>
     <row r="220">
       <c r="A220" t="n">
-        <v>153</v>
+        <v>195</v>
       </c>
       <c r="B220" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C220" t="n">
         <v>1</v>
@@ -6171,10 +6171,10 @@
     </row>
     <row r="221">
       <c r="A221" t="n">
-        <v>154</v>
+        <v>196</v>
       </c>
       <c r="B221" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C221" t="n">
         <v>1</v>
@@ -6197,7 +6197,7 @@
     </row>
     <row r="222">
       <c r="A222" t="n">
-        <v>155</v>
+        <v>197</v>
       </c>
       <c r="B222" t="n">
         <v>0</v>
@@ -6223,7 +6223,7 @@
     </row>
     <row r="223">
       <c r="A223" t="n">
-        <v>156</v>
+        <v>198</v>
       </c>
       <c r="B223" t="n">
         <v>0</v>
@@ -6249,7 +6249,7 @@
     </row>
     <row r="224">
       <c r="A224" t="n">
-        <v>157</v>
+        <v>199</v>
       </c>
       <c r="B224" t="n">
         <v>0</v>
@@ -6275,7 +6275,7 @@
     </row>
     <row r="225">
       <c r="A225" t="n">
-        <v>158</v>
+        <v>200</v>
       </c>
       <c r="B225" t="n">
         <v>0</v>
@@ -6301,7 +6301,7 @@
     </row>
     <row r="226">
       <c r="A226" t="n">
-        <v>159</v>
+        <v>201</v>
       </c>
       <c r="B226" t="n">
         <v>0</v>
@@ -6327,7 +6327,7 @@
     </row>
     <row r="227">
       <c r="A227" t="n">
-        <v>160</v>
+        <v>202</v>
       </c>
       <c r="B227" t="n">
         <v>0</v>
@@ -6353,7 +6353,7 @@
     </row>
     <row r="228">
       <c r="A228" t="n">
-        <v>161</v>
+        <v>203</v>
       </c>
       <c r="B228" t="n">
         <v>0</v>
@@ -6379,7 +6379,7 @@
     </row>
     <row r="229">
       <c r="A229" t="n">
-        <v>162</v>
+        <v>204</v>
       </c>
       <c r="B229" t="n">
         <v>0</v>
@@ -6405,7 +6405,7 @@
     </row>
     <row r="230">
       <c r="A230" t="n">
-        <v>163</v>
+        <v>205</v>
       </c>
       <c r="B230" t="n">
         <v>0</v>
@@ -6431,7 +6431,7 @@
     </row>
     <row r="231">
       <c r="A231" t="n">
-        <v>164</v>
+        <v>206</v>
       </c>
       <c r="B231" t="n">
         <v>0</v>
@@ -6457,7 +6457,7 @@
     </row>
     <row r="232">
       <c r="A232" t="n">
-        <v>165</v>
+        <v>207</v>
       </c>
       <c r="B232" t="n">
         <v>0</v>
@@ -6483,7 +6483,7 @@
     </row>
     <row r="233">
       <c r="A233" t="n">
-        <v>166</v>
+        <v>208</v>
       </c>
       <c r="B233" t="n">
         <v>0</v>
@@ -6509,7 +6509,7 @@
     </row>
     <row r="234">
       <c r="A234" t="n">
-        <v>167</v>
+        <v>209</v>
       </c>
       <c r="B234" t="n">
         <v>0</v>
@@ -6535,7 +6535,7 @@
     </row>
     <row r="235">
       <c r="A235" t="n">
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="B235" t="n">
         <v>0</v>
@@ -6561,7 +6561,7 @@
     </row>
     <row r="236">
       <c r="A236" t="n">
-        <v>169</v>
+        <v>211</v>
       </c>
       <c r="B236" t="n">
         <v>0</v>
@@ -6587,7 +6587,7 @@
     </row>
     <row r="237">
       <c r="A237" t="n">
-        <v>170</v>
+        <v>212</v>
       </c>
       <c r="B237" t="n">
         <v>0</v>
@@ -6613,7 +6613,7 @@
     </row>
     <row r="238">
       <c r="A238" t="n">
-        <v>171</v>
+        <v>213</v>
       </c>
       <c r="B238" t="n">
         <v>0</v>
@@ -6639,7 +6639,7 @@
     </row>
     <row r="239">
       <c r="A239" t="n">
-        <v>172</v>
+        <v>214</v>
       </c>
       <c r="B239" t="n">
         <v>0</v>
@@ -6665,7 +6665,7 @@
     </row>
     <row r="240">
       <c r="A240" t="n">
-        <v>173</v>
+        <v>215</v>
       </c>
       <c r="B240" t="n">
         <v>0</v>
@@ -6691,7 +6691,7 @@
     </row>
     <row r="241">
       <c r="A241" t="n">
-        <v>174</v>
+        <v>216</v>
       </c>
       <c r="B241" t="n">
         <v>0</v>
@@ -6717,7 +6717,7 @@
     </row>
     <row r="242">
       <c r="A242" t="n">
-        <v>175</v>
+        <v>217</v>
       </c>
       <c r="B242" t="n">
         <v>0</v>
@@ -6743,7 +6743,7 @@
     </row>
     <row r="243">
       <c r="A243" t="n">
-        <v>176</v>
+        <v>218</v>
       </c>
       <c r="B243" t="n">
         <v>0</v>
@@ -6769,7 +6769,7 @@
     </row>
     <row r="244">
       <c r="A244" t="n">
-        <v>177</v>
+        <v>219</v>
       </c>
       <c r="B244" t="n">
         <v>0</v>
@@ -6795,7 +6795,7 @@
     </row>
     <row r="245">
       <c r="A245" t="n">
-        <v>178</v>
+        <v>220</v>
       </c>
       <c r="B245" t="n">
         <v>0</v>
@@ -6821,7 +6821,7 @@
     </row>
     <row r="246">
       <c r="A246" t="n">
-        <v>179</v>
+        <v>221</v>
       </c>
       <c r="B246" t="n">
         <v>0</v>
@@ -6847,7 +6847,7 @@
     </row>
     <row r="247">
       <c r="A247" t="n">
-        <v>180</v>
+        <v>222</v>
       </c>
       <c r="B247" t="n">
         <v>0</v>
@@ -6873,7 +6873,7 @@
     </row>
     <row r="248">
       <c r="A248" t="n">
-        <v>181</v>
+        <v>223</v>
       </c>
       <c r="B248" t="n">
         <v>0</v>
@@ -6899,7 +6899,7 @@
     </row>
     <row r="249">
       <c r="A249" t="n">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="B249" t="n">
         <v>0</v>
@@ -6925,7 +6925,7 @@
     </row>
     <row r="250">
       <c r="A250" t="n">
-        <v>183</v>
+        <v>225</v>
       </c>
       <c r="B250" t="n">
         <v>0</v>
@@ -6951,7 +6951,7 @@
     </row>
     <row r="251">
       <c r="A251" t="n">
-        <v>184</v>
+        <v>226</v>
       </c>
       <c r="B251" t="n">
         <v>0</v>
@@ -6977,7 +6977,7 @@
     </row>
     <row r="252">
       <c r="A252" t="n">
-        <v>185</v>
+        <v>227</v>
       </c>
       <c r="B252" t="n">
         <v>0</v>
@@ -7003,7 +7003,7 @@
     </row>
     <row r="253">
       <c r="A253" t="n">
-        <v>186</v>
+        <v>228</v>
       </c>
       <c r="B253" t="n">
         <v>0</v>
@@ -7029,7 +7029,7 @@
     </row>
     <row r="254">
       <c r="A254" t="n">
-        <v>187</v>
+        <v>229</v>
       </c>
       <c r="B254" t="n">
         <v>0</v>
@@ -7055,7 +7055,7 @@
     </row>
     <row r="255">
       <c r="A255" t="n">
-        <v>188</v>
+        <v>230</v>
       </c>
       <c r="B255" t="n">
         <v>0</v>
@@ -7081,7 +7081,7 @@
     </row>
     <row r="256">
       <c r="A256" t="n">
-        <v>189</v>
+        <v>231</v>
       </c>
       <c r="B256" t="n">
         <v>0</v>
@@ -7107,7 +7107,7 @@
     </row>
     <row r="257">
       <c r="A257" t="n">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="B257" t="n">
         <v>0</v>
@@ -7133,7 +7133,7 @@
     </row>
     <row r="258">
       <c r="A258" t="n">
-        <v>191</v>
+        <v>233</v>
       </c>
       <c r="B258" t="n">
         <v>0</v>
@@ -7159,7 +7159,7 @@
     </row>
     <row r="259">
       <c r="A259" t="n">
-        <v>192</v>
+        <v>234</v>
       </c>
       <c r="B259" t="n">
         <v>0</v>
@@ -7185,7 +7185,7 @@
     </row>
     <row r="260">
       <c r="A260" t="n">
-        <v>193</v>
+        <v>235</v>
       </c>
       <c r="B260" t="n">
         <v>0</v>
@@ -7211,7 +7211,7 @@
     </row>
     <row r="261">
       <c r="A261" t="n">
-        <v>194</v>
+        <v>236</v>
       </c>
       <c r="B261" t="n">
         <v>0</v>
@@ -7237,7 +7237,7 @@
     </row>
     <row r="262">
       <c r="A262" t="n">
-        <v>195</v>
+        <v>237</v>
       </c>
       <c r="B262" t="n">
         <v>0</v>
@@ -7263,7 +7263,7 @@
     </row>
     <row r="263">
       <c r="A263" t="n">
-        <v>196</v>
+        <v>238</v>
       </c>
       <c r="B263" t="n">
         <v>0</v>
@@ -7289,7 +7289,7 @@
     </row>
     <row r="264">
       <c r="A264" t="n">
-        <v>197</v>
+        <v>239</v>
       </c>
       <c r="B264" t="n">
         <v>0</v>
@@ -7315,7 +7315,7 @@
     </row>
     <row r="265">
       <c r="A265" t="n">
-        <v>198</v>
+        <v>240</v>
       </c>
       <c r="B265" t="n">
         <v>0</v>
@@ -7341,7 +7341,7 @@
     </row>
     <row r="266">
       <c r="A266" t="n">
-        <v>199</v>
+        <v>241</v>
       </c>
       <c r="B266" t="n">
         <v>0</v>
@@ -7367,7 +7367,7 @@
     </row>
     <row r="267">
       <c r="A267" t="n">
-        <v>200</v>
+        <v>242</v>
       </c>
       <c r="B267" t="n">
         <v>0</v>
@@ -7393,7 +7393,7 @@
     </row>
     <row r="268">
       <c r="A268" t="n">
-        <v>201</v>
+        <v>243</v>
       </c>
       <c r="B268" t="n">
         <v>0</v>
@@ -7419,7 +7419,7 @@
     </row>
     <row r="269">
       <c r="A269" t="n">
-        <v>202</v>
+        <v>244</v>
       </c>
       <c r="B269" t="n">
         <v>0</v>
@@ -7445,7 +7445,7 @@
     </row>
     <row r="270">
       <c r="A270" t="n">
-        <v>203</v>
+        <v>245</v>
       </c>
       <c r="B270" t="n">
         <v>0</v>
@@ -7471,7 +7471,7 @@
     </row>
     <row r="271">
       <c r="A271" t="n">
-        <v>204</v>
+        <v>246</v>
       </c>
       <c r="B271" t="n">
         <v>0</v>
@@ -7497,7 +7497,7 @@
     </row>
     <row r="272">
       <c r="A272" t="n">
-        <v>205</v>
+        <v>247</v>
       </c>
       <c r="B272" t="n">
         <v>0</v>
@@ -7523,7 +7523,7 @@
     </row>
     <row r="273">
       <c r="A273" t="n">
-        <v>206</v>
+        <v>248</v>
       </c>
       <c r="B273" t="n">
         <v>0</v>
@@ -7549,7 +7549,7 @@
     </row>
     <row r="274">
       <c r="A274" t="n">
-        <v>207</v>
+        <v>249</v>
       </c>
       <c r="B274" t="n">
         <v>0</v>
@@ -7575,7 +7575,7 @@
     </row>
     <row r="275">
       <c r="A275" t="n">
-        <v>208</v>
+        <v>250</v>
       </c>
       <c r="B275" t="n">
         <v>0</v>
@@ -7601,7 +7601,7 @@
     </row>
     <row r="276">
       <c r="A276" t="n">
-        <v>209</v>
+        <v>251</v>
       </c>
       <c r="B276" t="n">
         <v>0</v>
@@ -7627,7 +7627,7 @@
     </row>
     <row r="277">
       <c r="A277" t="n">
-        <v>210</v>
+        <v>252</v>
       </c>
       <c r="B277" t="n">
         <v>0</v>
@@ -7653,7 +7653,7 @@
     </row>
     <row r="278">
       <c r="A278" t="n">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="B278" t="n">
         <v>0</v>
@@ -7679,7 +7679,7 @@
     </row>
     <row r="279">
       <c r="A279" t="n">
-        <v>212</v>
+        <v>254</v>
       </c>
       <c r="B279" t="n">
         <v>0</v>
@@ -7705,7 +7705,7 @@
     </row>
     <row r="280">
       <c r="A280" t="n">
-        <v>213</v>
+        <v>255</v>
       </c>
       <c r="B280" t="n">
         <v>0</v>
@@ -7731,7 +7731,7 @@
     </row>
     <row r="281">
       <c r="A281" t="n">
-        <v>214</v>
+        <v>256</v>
       </c>
       <c r="B281" t="n">
         <v>0</v>
@@ -7757,7 +7757,7 @@
     </row>
     <row r="282">
       <c r="A282" t="n">
-        <v>215</v>
+        <v>257</v>
       </c>
       <c r="B282" t="n">
         <v>0</v>
@@ -7783,7 +7783,7 @@
     </row>
     <row r="283">
       <c r="A283" t="n">
-        <v>216</v>
+        <v>258</v>
       </c>
       <c r="B283" t="n">
         <v>0</v>
@@ -7809,7 +7809,7 @@
     </row>
     <row r="284">
       <c r="A284" t="n">
-        <v>217</v>
+        <v>259</v>
       </c>
       <c r="B284" t="n">
         <v>0</v>
@@ -7835,7 +7835,7 @@
     </row>
     <row r="285">
       <c r="A285" t="n">
-        <v>218</v>
+        <v>260</v>
       </c>
       <c r="B285" t="n">
         <v>0</v>
@@ -7861,7 +7861,7 @@
     </row>
     <row r="286">
       <c r="A286" t="n">
-        <v>219</v>
+        <v>261</v>
       </c>
       <c r="B286" t="n">
         <v>0</v>
@@ -7887,7 +7887,7 @@
     </row>
     <row r="287">
       <c r="A287" t="n">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="B287" t="n">
         <v>0</v>
@@ -7913,7 +7913,7 @@
     </row>
     <row r="288">
       <c r="A288" t="n">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="B288" t="n">
         <v>0</v>
@@ -7939,7 +7939,7 @@
     </row>
     <row r="289">
       <c r="A289" t="n">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="B289" t="n">
         <v>0</v>
@@ -7965,7 +7965,7 @@
     </row>
     <row r="290">
       <c r="A290" t="n">
-        <v>223</v>
+        <v>265</v>
       </c>
       <c r="B290" t="n">
         <v>0</v>
@@ -7991,7 +7991,7 @@
     </row>
     <row r="291">
       <c r="A291" t="n">
-        <v>224</v>
+        <v>266</v>
       </c>
       <c r="B291" t="n">
         <v>0</v>
@@ -8017,7 +8017,7 @@
     </row>
     <row r="292">
       <c r="A292" t="n">
-        <v>225</v>
+        <v>267</v>
       </c>
       <c r="B292" t="n">
         <v>0</v>
@@ -8043,7 +8043,7 @@
     </row>
     <row r="293">
       <c r="A293" t="n">
-        <v>226</v>
+        <v>268</v>
       </c>
       <c r="B293" t="n">
         <v>0</v>
@@ -8069,7 +8069,7 @@
     </row>
     <row r="294">
       <c r="A294" t="n">
-        <v>227</v>
+        <v>269</v>
       </c>
       <c r="B294" t="n">
         <v>0</v>
@@ -8095,7 +8095,7 @@
     </row>
     <row r="295">
       <c r="A295" t="n">
-        <v>228</v>
+        <v>270</v>
       </c>
       <c r="B295" t="n">
         <v>0</v>
@@ -8121,7 +8121,7 @@
     </row>
     <row r="296">
       <c r="A296" t="n">
-        <v>229</v>
+        <v>271</v>
       </c>
       <c r="B296" t="n">
         <v>0</v>
@@ -8147,7 +8147,7 @@
     </row>
     <row r="297">
       <c r="A297" t="n">
-        <v>230</v>
+        <v>272</v>
       </c>
       <c r="B297" t="n">
         <v>0</v>
@@ -8173,7 +8173,7 @@
     </row>
     <row r="298">
       <c r="A298" t="n">
-        <v>231</v>
+        <v>273</v>
       </c>
       <c r="B298" t="n">
         <v>0</v>
@@ -8199,7 +8199,7 @@
     </row>
     <row r="299">
       <c r="A299" t="n">
-        <v>232</v>
+        <v>274</v>
       </c>
       <c r="B299" t="n">
         <v>0</v>
@@ -8225,7 +8225,7 @@
     </row>
     <row r="300">
       <c r="A300" t="n">
-        <v>233</v>
+        <v>275</v>
       </c>
       <c r="B300" t="n">
         <v>0</v>
@@ -8251,7 +8251,7 @@
     </row>
     <row r="301">
       <c r="A301" t="n">
-        <v>234</v>
+        <v>276</v>
       </c>
       <c r="B301" t="n">
         <v>0</v>
@@ -8277,7 +8277,7 @@
     </row>
     <row r="302">
       <c r="A302" t="n">
-        <v>235</v>
+        <v>277</v>
       </c>
       <c r="B302" t="n">
         <v>0</v>
@@ -8303,7 +8303,7 @@
     </row>
     <row r="303">
       <c r="A303" t="n">
-        <v>236</v>
+        <v>278</v>
       </c>
       <c r="B303" t="n">
         <v>0</v>
@@ -8329,7 +8329,7 @@
     </row>
     <row r="304">
       <c r="A304" t="n">
-        <v>237</v>
+        <v>279</v>
       </c>
       <c r="B304" t="n">
         <v>0</v>
@@ -8355,7 +8355,7 @@
     </row>
     <row r="305">
       <c r="A305" t="n">
-        <v>238</v>
+        <v>280</v>
       </c>
       <c r="B305" t="n">
         <v>0</v>
@@ -8381,7 +8381,7 @@
     </row>
     <row r="306">
       <c r="A306" t="n">
-        <v>239</v>
+        <v>281</v>
       </c>
       <c r="B306" t="n">
         <v>0</v>
@@ -8407,7 +8407,7 @@
     </row>
     <row r="307">
       <c r="A307" t="n">
-        <v>240</v>
+        <v>282</v>
       </c>
       <c r="B307" t="n">
         <v>0</v>
@@ -8433,7 +8433,7 @@
     </row>
     <row r="308">
       <c r="A308" t="n">
-        <v>241</v>
+        <v>283</v>
       </c>
       <c r="B308" t="n">
         <v>0</v>
@@ -8459,7 +8459,7 @@
     </row>
     <row r="309">
       <c r="A309" t="n">
-        <v>242</v>
+        <v>284</v>
       </c>
       <c r="B309" t="n">
         <v>0</v>
@@ -8485,7 +8485,7 @@
     </row>
     <row r="310">
       <c r="A310" t="n">
-        <v>243</v>
+        <v>285</v>
       </c>
       <c r="B310" t="n">
         <v>0</v>
@@ -8511,7 +8511,7 @@
     </row>
     <row r="311">
       <c r="A311" t="n">
-        <v>244</v>
+        <v>286</v>
       </c>
       <c r="B311" t="n">
         <v>0</v>
@@ -8537,7 +8537,7 @@
     </row>
     <row r="312">
       <c r="A312" t="n">
-        <v>245</v>
+        <v>287</v>
       </c>
       <c r="B312" t="n">
         <v>0</v>
@@ -8563,7 +8563,7 @@
     </row>
     <row r="313">
       <c r="A313" t="n">
-        <v>246</v>
+        <v>288</v>
       </c>
       <c r="B313" t="n">
         <v>0</v>
@@ -8589,7 +8589,7 @@
     </row>
     <row r="314">
       <c r="A314" t="n">
-        <v>247</v>
+        <v>289</v>
       </c>
       <c r="B314" t="n">
         <v>0</v>
@@ -8615,7 +8615,7 @@
     </row>
     <row r="315">
       <c r="A315" t="n">
-        <v>248</v>
+        <v>290</v>
       </c>
       <c r="B315" t="n">
         <v>0</v>
@@ -8641,7 +8641,7 @@
     </row>
     <row r="316">
       <c r="A316" t="n">
-        <v>249</v>
+        <v>291</v>
       </c>
       <c r="B316" t="n">
         <v>0</v>
@@ -8662,1098 +8662,6 @@
         <v>0.9</v>
       </c>
       <c r="H316" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="317">
-      <c r="A317" t="n">
-        <v>250</v>
-      </c>
-      <c r="B317" t="n">
-        <v>0</v>
-      </c>
-      <c r="C317" t="n">
-        <v>1</v>
-      </c>
-      <c r="D317" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E317" t="n">
-        <v>1</v>
-      </c>
-      <c r="F317" t="n">
-        <v>1</v>
-      </c>
-      <c r="G317" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H317" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="318">
-      <c r="A318" t="n">
-        <v>251</v>
-      </c>
-      <c r="B318" t="n">
-        <v>0</v>
-      </c>
-      <c r="C318" t="n">
-        <v>1</v>
-      </c>
-      <c r="D318" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E318" t="n">
-        <v>1</v>
-      </c>
-      <c r="F318" t="n">
-        <v>1</v>
-      </c>
-      <c r="G318" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H318" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="319">
-      <c r="A319" t="n">
-        <v>252</v>
-      </c>
-      <c r="B319" t="n">
-        <v>0</v>
-      </c>
-      <c r="C319" t="n">
-        <v>1</v>
-      </c>
-      <c r="D319" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E319" t="n">
-        <v>1</v>
-      </c>
-      <c r="F319" t="n">
-        <v>1</v>
-      </c>
-      <c r="G319" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H319" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="320">
-      <c r="A320" t="n">
-        <v>253</v>
-      </c>
-      <c r="B320" t="n">
-        <v>0</v>
-      </c>
-      <c r="C320" t="n">
-        <v>1</v>
-      </c>
-      <c r="D320" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E320" t="n">
-        <v>1</v>
-      </c>
-      <c r="F320" t="n">
-        <v>1</v>
-      </c>
-      <c r="G320" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H320" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="321">
-      <c r="A321" t="n">
-        <v>254</v>
-      </c>
-      <c r="B321" t="n">
-        <v>0</v>
-      </c>
-      <c r="C321" t="n">
-        <v>1</v>
-      </c>
-      <c r="D321" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E321" t="n">
-        <v>1</v>
-      </c>
-      <c r="F321" t="n">
-        <v>1</v>
-      </c>
-      <c r="G321" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H321" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="322">
-      <c r="A322" t="n">
-        <v>255</v>
-      </c>
-      <c r="B322" t="n">
-        <v>0</v>
-      </c>
-      <c r="C322" t="n">
-        <v>1</v>
-      </c>
-      <c r="D322" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E322" t="n">
-        <v>1</v>
-      </c>
-      <c r="F322" t="n">
-        <v>1</v>
-      </c>
-      <c r="G322" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H322" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="323">
-      <c r="A323" t="n">
-        <v>256</v>
-      </c>
-      <c r="B323" t="n">
-        <v>0</v>
-      </c>
-      <c r="C323" t="n">
-        <v>1</v>
-      </c>
-      <c r="D323" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E323" t="n">
-        <v>1</v>
-      </c>
-      <c r="F323" t="n">
-        <v>1</v>
-      </c>
-      <c r="G323" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H323" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="324">
-      <c r="A324" t="n">
-        <v>257</v>
-      </c>
-      <c r="B324" t="n">
-        <v>0</v>
-      </c>
-      <c r="C324" t="n">
-        <v>1</v>
-      </c>
-      <c r="D324" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E324" t="n">
-        <v>1</v>
-      </c>
-      <c r="F324" t="n">
-        <v>1</v>
-      </c>
-      <c r="G324" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H324" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="325">
-      <c r="A325" t="n">
-        <v>258</v>
-      </c>
-      <c r="B325" t="n">
-        <v>0</v>
-      </c>
-      <c r="C325" t="n">
-        <v>1</v>
-      </c>
-      <c r="D325" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E325" t="n">
-        <v>1</v>
-      </c>
-      <c r="F325" t="n">
-        <v>1</v>
-      </c>
-      <c r="G325" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H325" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="326">
-      <c r="A326" t="n">
-        <v>259</v>
-      </c>
-      <c r="B326" t="n">
-        <v>0</v>
-      </c>
-      <c r="C326" t="n">
-        <v>1</v>
-      </c>
-      <c r="D326" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E326" t="n">
-        <v>1</v>
-      </c>
-      <c r="F326" t="n">
-        <v>1</v>
-      </c>
-      <c r="G326" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H326" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="327">
-      <c r="A327" t="n">
-        <v>260</v>
-      </c>
-      <c r="B327" t="n">
-        <v>0</v>
-      </c>
-      <c r="C327" t="n">
-        <v>1</v>
-      </c>
-      <c r="D327" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E327" t="n">
-        <v>1</v>
-      </c>
-      <c r="F327" t="n">
-        <v>1</v>
-      </c>
-      <c r="G327" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H327" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="328">
-      <c r="A328" t="n">
-        <v>261</v>
-      </c>
-      <c r="B328" t="n">
-        <v>0</v>
-      </c>
-      <c r="C328" t="n">
-        <v>1</v>
-      </c>
-      <c r="D328" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E328" t="n">
-        <v>1</v>
-      </c>
-      <c r="F328" t="n">
-        <v>1</v>
-      </c>
-      <c r="G328" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H328" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="329">
-      <c r="A329" t="n">
-        <v>262</v>
-      </c>
-      <c r="B329" t="n">
-        <v>0</v>
-      </c>
-      <c r="C329" t="n">
-        <v>1</v>
-      </c>
-      <c r="D329" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E329" t="n">
-        <v>1</v>
-      </c>
-      <c r="F329" t="n">
-        <v>1</v>
-      </c>
-      <c r="G329" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H329" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="330">
-      <c r="A330" t="n">
-        <v>263</v>
-      </c>
-      <c r="B330" t="n">
-        <v>0</v>
-      </c>
-      <c r="C330" t="n">
-        <v>1</v>
-      </c>
-      <c r="D330" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E330" t="n">
-        <v>1</v>
-      </c>
-      <c r="F330" t="n">
-        <v>1</v>
-      </c>
-      <c r="G330" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H330" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="331">
-      <c r="A331" t="n">
-        <v>264</v>
-      </c>
-      <c r="B331" t="n">
-        <v>0</v>
-      </c>
-      <c r="C331" t="n">
-        <v>1</v>
-      </c>
-      <c r="D331" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E331" t="n">
-        <v>1</v>
-      </c>
-      <c r="F331" t="n">
-        <v>1</v>
-      </c>
-      <c r="G331" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H331" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="332">
-      <c r="A332" t="n">
-        <v>265</v>
-      </c>
-      <c r="B332" t="n">
-        <v>0</v>
-      </c>
-      <c r="C332" t="n">
-        <v>1</v>
-      </c>
-      <c r="D332" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E332" t="n">
-        <v>1</v>
-      </c>
-      <c r="F332" t="n">
-        <v>1</v>
-      </c>
-      <c r="G332" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H332" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="333">
-      <c r="A333" t="n">
-        <v>266</v>
-      </c>
-      <c r="B333" t="n">
-        <v>0</v>
-      </c>
-      <c r="C333" t="n">
-        <v>1</v>
-      </c>
-      <c r="D333" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E333" t="n">
-        <v>1</v>
-      </c>
-      <c r="F333" t="n">
-        <v>1</v>
-      </c>
-      <c r="G333" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H333" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="334">
-      <c r="A334" t="n">
-        <v>267</v>
-      </c>
-      <c r="B334" t="n">
-        <v>0</v>
-      </c>
-      <c r="C334" t="n">
-        <v>1</v>
-      </c>
-      <c r="D334" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E334" t="n">
-        <v>1</v>
-      </c>
-      <c r="F334" t="n">
-        <v>1</v>
-      </c>
-      <c r="G334" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H334" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="335">
-      <c r="A335" t="n">
-        <v>268</v>
-      </c>
-      <c r="B335" t="n">
-        <v>0</v>
-      </c>
-      <c r="C335" t="n">
-        <v>1</v>
-      </c>
-      <c r="D335" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E335" t="n">
-        <v>1</v>
-      </c>
-      <c r="F335" t="n">
-        <v>1</v>
-      </c>
-      <c r="G335" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H335" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="336">
-      <c r="A336" t="n">
-        <v>269</v>
-      </c>
-      <c r="B336" t="n">
-        <v>0</v>
-      </c>
-      <c r="C336" t="n">
-        <v>1</v>
-      </c>
-      <c r="D336" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E336" t="n">
-        <v>1</v>
-      </c>
-      <c r="F336" t="n">
-        <v>1</v>
-      </c>
-      <c r="G336" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H336" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="337">
-      <c r="A337" t="n">
-        <v>270</v>
-      </c>
-      <c r="B337" t="n">
-        <v>0</v>
-      </c>
-      <c r="C337" t="n">
-        <v>1</v>
-      </c>
-      <c r="D337" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E337" t="n">
-        <v>1</v>
-      </c>
-      <c r="F337" t="n">
-        <v>1</v>
-      </c>
-      <c r="G337" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H337" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="338">
-      <c r="A338" t="n">
-        <v>271</v>
-      </c>
-      <c r="B338" t="n">
-        <v>0</v>
-      </c>
-      <c r="C338" t="n">
-        <v>1</v>
-      </c>
-      <c r="D338" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E338" t="n">
-        <v>1</v>
-      </c>
-      <c r="F338" t="n">
-        <v>1</v>
-      </c>
-      <c r="G338" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H338" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="339">
-      <c r="A339" t="n">
-        <v>272</v>
-      </c>
-      <c r="B339" t="n">
-        <v>0</v>
-      </c>
-      <c r="C339" t="n">
-        <v>1</v>
-      </c>
-      <c r="D339" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E339" t="n">
-        <v>1</v>
-      </c>
-      <c r="F339" t="n">
-        <v>1</v>
-      </c>
-      <c r="G339" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H339" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="340">
-      <c r="A340" t="n">
-        <v>273</v>
-      </c>
-      <c r="B340" t="n">
-        <v>0</v>
-      </c>
-      <c r="C340" t="n">
-        <v>1</v>
-      </c>
-      <c r="D340" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E340" t="n">
-        <v>1</v>
-      </c>
-      <c r="F340" t="n">
-        <v>1</v>
-      </c>
-      <c r="G340" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H340" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="341">
-      <c r="A341" t="n">
-        <v>274</v>
-      </c>
-      <c r="B341" t="n">
-        <v>0</v>
-      </c>
-      <c r="C341" t="n">
-        <v>1</v>
-      </c>
-      <c r="D341" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E341" t="n">
-        <v>1</v>
-      </c>
-      <c r="F341" t="n">
-        <v>1</v>
-      </c>
-      <c r="G341" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H341" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="342">
-      <c r="A342" t="n">
-        <v>275</v>
-      </c>
-      <c r="B342" t="n">
-        <v>0</v>
-      </c>
-      <c r="C342" t="n">
-        <v>1</v>
-      </c>
-      <c r="D342" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E342" t="n">
-        <v>1</v>
-      </c>
-      <c r="F342" t="n">
-        <v>1</v>
-      </c>
-      <c r="G342" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H342" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="343">
-      <c r="A343" t="n">
-        <v>276</v>
-      </c>
-      <c r="B343" t="n">
-        <v>0</v>
-      </c>
-      <c r="C343" t="n">
-        <v>1</v>
-      </c>
-      <c r="D343" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E343" t="n">
-        <v>1</v>
-      </c>
-      <c r="F343" t="n">
-        <v>1</v>
-      </c>
-      <c r="G343" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H343" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="344">
-      <c r="A344" t="n">
-        <v>277</v>
-      </c>
-      <c r="B344" t="n">
-        <v>0</v>
-      </c>
-      <c r="C344" t="n">
-        <v>1</v>
-      </c>
-      <c r="D344" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E344" t="n">
-        <v>1</v>
-      </c>
-      <c r="F344" t="n">
-        <v>1</v>
-      </c>
-      <c r="G344" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H344" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="345">
-      <c r="A345" t="n">
-        <v>278</v>
-      </c>
-      <c r="B345" t="n">
-        <v>0</v>
-      </c>
-      <c r="C345" t="n">
-        <v>1</v>
-      </c>
-      <c r="D345" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E345" t="n">
-        <v>1</v>
-      </c>
-      <c r="F345" t="n">
-        <v>1</v>
-      </c>
-      <c r="G345" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H345" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="346">
-      <c r="A346" t="n">
-        <v>279</v>
-      </c>
-      <c r="B346" t="n">
-        <v>0</v>
-      </c>
-      <c r="C346" t="n">
-        <v>1</v>
-      </c>
-      <c r="D346" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E346" t="n">
-        <v>1</v>
-      </c>
-      <c r="F346" t="n">
-        <v>1</v>
-      </c>
-      <c r="G346" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H346" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="347">
-      <c r="A347" t="n">
-        <v>280</v>
-      </c>
-      <c r="B347" t="n">
-        <v>0</v>
-      </c>
-      <c r="C347" t="n">
-        <v>1</v>
-      </c>
-      <c r="D347" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E347" t="n">
-        <v>1</v>
-      </c>
-      <c r="F347" t="n">
-        <v>1</v>
-      </c>
-      <c r="G347" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H347" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="348">
-      <c r="A348" t="n">
-        <v>281</v>
-      </c>
-      <c r="B348" t="n">
-        <v>0</v>
-      </c>
-      <c r="C348" t="n">
-        <v>1</v>
-      </c>
-      <c r="D348" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E348" t="n">
-        <v>1</v>
-      </c>
-      <c r="F348" t="n">
-        <v>1</v>
-      </c>
-      <c r="G348" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H348" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="349">
-      <c r="A349" t="n">
-        <v>282</v>
-      </c>
-      <c r="B349" t="n">
-        <v>0</v>
-      </c>
-      <c r="C349" t="n">
-        <v>1</v>
-      </c>
-      <c r="D349" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E349" t="n">
-        <v>1</v>
-      </c>
-      <c r="F349" t="n">
-        <v>1</v>
-      </c>
-      <c r="G349" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H349" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="350">
-      <c r="A350" t="n">
-        <v>283</v>
-      </c>
-      <c r="B350" t="n">
-        <v>0</v>
-      </c>
-      <c r="C350" t="n">
-        <v>1</v>
-      </c>
-      <c r="D350" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E350" t="n">
-        <v>1</v>
-      </c>
-      <c r="F350" t="n">
-        <v>1</v>
-      </c>
-      <c r="G350" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H350" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="351">
-      <c r="A351" t="n">
-        <v>284</v>
-      </c>
-      <c r="B351" t="n">
-        <v>0</v>
-      </c>
-      <c r="C351" t="n">
-        <v>1</v>
-      </c>
-      <c r="D351" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E351" t="n">
-        <v>1</v>
-      </c>
-      <c r="F351" t="n">
-        <v>1</v>
-      </c>
-      <c r="G351" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H351" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="352">
-      <c r="A352" t="n">
-        <v>285</v>
-      </c>
-      <c r="B352" t="n">
-        <v>0</v>
-      </c>
-      <c r="C352" t="n">
-        <v>1</v>
-      </c>
-      <c r="D352" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E352" t="n">
-        <v>1</v>
-      </c>
-      <c r="F352" t="n">
-        <v>1</v>
-      </c>
-      <c r="G352" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H352" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="353">
-      <c r="A353" t="n">
-        <v>286</v>
-      </c>
-      <c r="B353" t="n">
-        <v>0</v>
-      </c>
-      <c r="C353" t="n">
-        <v>1</v>
-      </c>
-      <c r="D353" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E353" t="n">
-        <v>1</v>
-      </c>
-      <c r="F353" t="n">
-        <v>1</v>
-      </c>
-      <c r="G353" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H353" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="354">
-      <c r="A354" t="n">
-        <v>287</v>
-      </c>
-      <c r="B354" t="n">
-        <v>0</v>
-      </c>
-      <c r="C354" t="n">
-        <v>1</v>
-      </c>
-      <c r="D354" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E354" t="n">
-        <v>1</v>
-      </c>
-      <c r="F354" t="n">
-        <v>1</v>
-      </c>
-      <c r="G354" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H354" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="355">
-      <c r="A355" t="n">
-        <v>288</v>
-      </c>
-      <c r="B355" t="n">
-        <v>0</v>
-      </c>
-      <c r="C355" t="n">
-        <v>1</v>
-      </c>
-      <c r="D355" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E355" t="n">
-        <v>1</v>
-      </c>
-      <c r="F355" t="n">
-        <v>1</v>
-      </c>
-      <c r="G355" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H355" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="356">
-      <c r="A356" t="n">
-        <v>289</v>
-      </c>
-      <c r="B356" t="n">
-        <v>0</v>
-      </c>
-      <c r="C356" t="n">
-        <v>1</v>
-      </c>
-      <c r="D356" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E356" t="n">
-        <v>1</v>
-      </c>
-      <c r="F356" t="n">
-        <v>1</v>
-      </c>
-      <c r="G356" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H356" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="357">
-      <c r="A357" t="n">
-        <v>290</v>
-      </c>
-      <c r="B357" t="n">
-        <v>0</v>
-      </c>
-      <c r="C357" t="n">
-        <v>1</v>
-      </c>
-      <c r="D357" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E357" t="n">
-        <v>1</v>
-      </c>
-      <c r="F357" t="n">
-        <v>1</v>
-      </c>
-      <c r="G357" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H357" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="358">
-      <c r="A358" t="n">
-        <v>291</v>
-      </c>
-      <c r="B358" t="n">
-        <v>0</v>
-      </c>
-      <c r="C358" t="n">
-        <v>1</v>
-      </c>
-      <c r="D358" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="E358" t="n">
-        <v>1</v>
-      </c>
-      <c r="F358" t="n">
-        <v>1</v>
-      </c>
-      <c r="G358" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H358" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>